<commit_message>
tidying up spm excel sheets
</commit_message>
<xml_diff>
--- a/Results/Plot data/ipcc_ar6_figure_spm_sectors.xlsx
+++ b/Results/Plot data/ipcc_ar6_figure_spm_sectors.xlsx
@@ -6,23 +6,54 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="direct emissions" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="indirect emissions" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="indirect emissions - subsectors" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="info" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="direct emissions" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="indirect emissions" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="indirect emissions - subsectors" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+  <si>
+    <t xml:space="preserve">Author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">William F. Lamb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-10-14 10:09:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/mcc-apsis/AR6-Emissions-trends-and-drivers/blob/master/R/Analysis%20and%20figures/direct_indirect_emissions.Rmd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GHG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GtCO2eq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
   <si>
     <t xml:space="preserve">chapter_title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GHG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fraction</t>
   </si>
   <si>
     <t xml:space="preserve">AFOLU</t>
@@ -553,74 +584,53 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="n">
-        <v>12.9775309663637</v>
-      </c>
-      <c r="C2" t="n">
-        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
-        <v>3.30326626886358</v>
-      </c>
-      <c r="C3" t="n">
-        <v>5.6</v>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="n">
-        <v>13.8392696618948</v>
-      </c>
-      <c r="C4" t="n">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="n">
-        <v>6.14027662374651</v>
-      </c>
-      <c r="C5" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="n">
-        <v>14.1122057326628</v>
-      </c>
-      <c r="C6" t="n">
-        <v>24</v>
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="n">
-        <v>8.71807557408101</v>
-      </c>
-      <c r="C7" t="n">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -639,187 +649,79 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="B2" t="n">
+        <v>12.9775309663637</v>
       </c>
       <c r="C2" t="n">
-        <v>6.14027662374651</v>
-      </c>
-      <c r="D2" t="n">
-        <v>7.30198040499617</v>
-      </c>
-      <c r="E2" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3.30326626886358</v>
       </c>
       <c r="C3" t="n">
-        <v>1.16170378124966</v>
-      </c>
-      <c r="D3" t="n">
-        <v>7.30198040499617</v>
-      </c>
-      <c r="E3" t="n">
-        <v>12</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B4" t="n">
+        <v>13.8392696618948</v>
       </c>
       <c r="C4" t="n">
-        <v>14.1122057326628</v>
-      </c>
-      <c r="D4" t="n">
-        <v>20.0253905011338</v>
-      </c>
-      <c r="E4" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6.14027662374651</v>
       </c>
       <c r="C5" t="n">
-        <v>5.91318476847108</v>
-      </c>
-      <c r="D5" t="n">
-        <v>20.0253905011338</v>
-      </c>
-      <c r="E5" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B6" t="n">
+        <v>14.1122057326628</v>
       </c>
       <c r="C6" t="n">
-        <v>12.9775309663637</v>
-      </c>
-      <c r="D6" t="n">
-        <v>12.9775309663637</v>
-      </c>
-      <c r="E6" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7"/>
-      <c r="D7" t="n">
-        <v>12.9775309663637</v>
-      </c>
-      <c r="E7" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
+        <v>18</v>
+      </c>
+      <c r="B7" t="n">
         <v>8.71807557408101</v>
       </c>
-      <c r="D8" t="n">
-        <v>8.94136614586484</v>
-      </c>
-      <c r="E8" t="n">
+      <c r="C7" t="n">
         <v>15</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.223290571783821</v>
-      </c>
-      <c r="D9" t="n">
-        <v>8.94136614586484</v>
-      </c>
-      <c r="E9" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>3.30326626886358</v>
-      </c>
-      <c r="D10" t="n">
-        <v>9.74786893235828</v>
-      </c>
-      <c r="E10" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="n">
-        <v>6.4446026634947</v>
-      </c>
-      <c r="D11" t="n">
-        <v>9.74786893235828</v>
-      </c>
-      <c r="E11" t="n">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -841,19 +743,218 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6.14027662374651</v>
+      </c>
+      <c r="D2" t="n">
+        <v>7.30198040499617</v>
+      </c>
+      <c r="E2" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.16170378124966</v>
+      </c>
+      <c r="D3" t="n">
+        <v>7.30198040499617</v>
+      </c>
+      <c r="E3" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>14.1122057326628</v>
+      </c>
+      <c r="D4" t="n">
+        <v>20.0253905011338</v>
+      </c>
+      <c r="E4" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5.91318476847108</v>
+      </c>
+      <c r="D5" t="n">
+        <v>20.0253905011338</v>
+      </c>
+      <c r="E5" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="n">
+        <v>12.9775309663637</v>
+      </c>
+      <c r="D6" t="n">
+        <v>12.9775309663637</v>
+      </c>
+      <c r="E6" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7" t="n">
+        <v>12.9775309663637</v>
+      </c>
+      <c r="E7" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8.71807557408101</v>
+      </c>
+      <c r="D8" t="n">
+        <v>8.94136614586484</v>
+      </c>
+      <c r="E8" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.223290571783821</v>
+      </c>
+      <c r="D9" t="n">
+        <v>8.94136614586484</v>
+      </c>
+      <c r="E9" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.30326626886358</v>
+      </c>
+      <c r="D10" t="n">
+        <v>9.74786893235828</v>
+      </c>
+      <c r="E10" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="n">
+        <v>6.4446026634947</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9.74786893235828</v>
+      </c>
+      <c r="E11" t="n">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2">
@@ -861,10 +962,10 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D2" t="n">
         <v>0.629138706260922</v>
@@ -873,7 +974,7 @@
         <v>1.1</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
@@ -881,10 +982,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D3" t="n">
         <v>1.27885470039701</v>
@@ -893,7 +994,7 @@
         <v>2.2</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
@@ -901,10 +1002,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D4" t="n">
         <v>2.62003212670528</v>
@@ -913,7 +1014,7 @@
         <v>4.4</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
@@ -921,10 +1022,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D5" t="n">
         <v>2.77395487163296</v>
@@ -933,7 +1034,7 @@
         <v>4.7</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -941,10 +1042,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D6" t="n">
         <v>1.5483146679</v>
@@ -953,7 +1054,7 @@
         <v>2.6</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
@@ -961,10 +1062,10 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D7" t="n">
         <v>2.32670399008267</v>
@@ -973,7 +1074,7 @@
         <v>3.9</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
@@ -981,10 +1082,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D8" t="n">
         <v>3.70068510843741</v>
@@ -993,7 +1094,7 @@
         <v>6.3</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9">
@@ -1001,10 +1102,10 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D9" t="n">
         <v>4.59677161771698</v>
@@ -1013,7 +1114,7 @@
         <v>7.8</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -1021,10 +1122,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D10" t="n">
         <v>7.85291511699677</v>
@@ -1033,7 +1134,7 @@
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -1041,10 +1142,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D11" t="n">
         <v>0.0682785057617064</v>
@@ -1053,7 +1154,7 @@
         <v>0.12</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
@@ -1061,10 +1162,10 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D12" t="n">
         <v>0.426016532913334</v>
@@ -1073,7 +1174,7 @@
         <v>0.72</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
@@ -1081,10 +1182,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D13" t="n">
         <v>0.443006868072477</v>
@@ -1093,7 +1194,7 @@
         <v>0.75</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14">
@@ -1101,10 +1202,10 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D14" t="n">
         <v>1.01757779807094</v>
@@ -1113,7 +1214,7 @@
         <v>1.7</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15">
@@ -1121,10 +1222,10 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D15" t="n">
         <v>1.45580903462043</v>
@@ -1133,7 +1234,7 @@
         <v>2.5</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
@@ -1141,10 +1242,10 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D16" t="n">
         <v>2.96180337932477</v>
@@ -1153,7 +1254,7 @@
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
@@ -1161,10 +1262,10 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D17" t="n">
         <v>6.6050388476</v>
@@ -1173,7 +1274,7 @@
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18">
@@ -1181,10 +1282,10 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="D18" t="n">
         <v>0.176709821781149</v>
@@ -1193,7 +1294,7 @@
         <v>0.3</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19">
@@ -1201,10 +1302,10 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D19" t="n">
         <v>0.253872814464669</v>
@@ -1213,7 +1314,7 @@
         <v>0.43</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20">
@@ -1221,10 +1322,10 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D20" t="n">
         <v>0.394138112810141</v>
@@ -1233,7 +1334,7 @@
         <v>0.67</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21">
@@ -1241,10 +1342,10 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D21" t="n">
         <v>0.532234093251387</v>
@@ -1253,7 +1354,7 @@
         <v>0.9</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22">
@@ -1261,10 +1362,10 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="D22" t="n">
         <v>0.620824495451895</v>
@@ -1273,7 +1374,7 @@
         <v>1.1</v>
       </c>
       <c r="F22" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23">
@@ -1281,10 +1382,10 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D23" t="n">
         <v>0.780617168336543</v>
@@ -1293,7 +1394,7 @@
         <v>1.3</v>
       </c>
       <c r="F23" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24">
@@ -1301,10 +1402,10 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D24" t="n">
         <v>6.18296963976905</v>
@@ -1313,7 +1414,7 @@
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25">
@@ -1321,10 +1422,10 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D25" t="n">
         <v>0.0428828735760605</v>
@@ -1333,7 +1434,7 @@
         <v>0.073</v>
       </c>
       <c r="F25" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26">
@@ -1341,10 +1442,10 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D26" t="n">
         <v>3.45280160975202</v>
@@ -1353,7 +1454,7 @@
         <v>5.9</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27">
@@ -1361,10 +1462,10 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D27" t="n">
         <v>6.2521844490302</v>
@@ -1373,7 +1474,7 @@
         <v>11</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>